<commit_message>
updated evaluation and info
</commit_message>
<xml_diff>
--- a/blocs/incentives/incentives_info.xlsx
+++ b/blocs/incentives/incentives_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39488DE7-B7F4-B341-A560-A0257FC2F2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A553CE-6E3B-0348-9650-1188BE2B873B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
@@ -689,7 +689,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
improve inc implementation, delete unnecessary files
Improved the implementation of tax incentives by making sure the biorefinery receives them during years which they pay tax. Removed unnecesssary/outdated files.
</commit_message>
<xml_diff>
--- a/blocs/incentives/incentives_info.xlsx
+++ b/blocs/incentives/incentives_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A553CE-6E3B-0348-9650-1188BE2B873B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF81A2-14DE-B549-8426-ADA425BBDC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
   <si>
     <t>property</t>
   </si>
@@ -41,9 +41,6 @@
     <t>motor fuel</t>
   </si>
   <si>
-    <t>utility</t>
-  </si>
-  <si>
     <t>income</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>Biofuel Production Facility Tax Exemption</t>
   </si>
   <si>
-    <t>Alternative Fuel Development Property Tax Exemption</t>
-  </si>
-  <si>
     <t>Ethanol Production Facility Property Tax Exemption</t>
   </si>
   <si>
@@ -119,27 +113,18 @@
     <t>Green Jobs Tax Credit</t>
   </si>
   <si>
-    <t>Second Generation Biofuel Producer Tax Credit</t>
-  </si>
-  <si>
     <t>Alternative Fuel Production Tax Incentives (KEIA)</t>
   </si>
   <si>
     <t>Ethanol Production Incentive</t>
   </si>
   <si>
-    <t>Second Generation Biofuel Plant Depreciation Deduction Allowance</t>
-  </si>
-  <si>
     <t>IA</t>
   </si>
   <si>
     <t>KS</t>
   </si>
   <si>
-    <t>MI</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -173,9 +158,6 @@
     <t>VA</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
@@ -197,9 +179,6 @@
     <t>array</t>
   </si>
   <si>
-    <t>biodiesel_eq</t>
-  </si>
-  <si>
     <t>ethanol_eq</t>
   </si>
   <si>
@@ -209,9 +188,6 @@
     <t>NM_value</t>
   </si>
   <si>
-    <t>wages</t>
-  </si>
-  <si>
     <t>TCI</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
   </si>
   <si>
     <t>corn or cellulosic feedstock only</t>
-  </si>
-  <si>
-    <t>second generation feedstocks only</t>
   </si>
   <si>
     <t>grain feedstock only</t>
@@ -689,7 +662,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I26" sqref="A22:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,31 +681,31 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="4"/>
@@ -742,28 +715,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -774,28 +747,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -805,25 +778,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J4" s="2"/>
       <c r="L4" s="5"/>
@@ -834,25 +807,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="M5" s="5"/>
     </row>
@@ -861,28 +834,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -891,25 +864,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="J7" s="2"/>
       <c r="L7" s="4"/>
@@ -921,25 +894,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M8" s="3"/>
     </row>
@@ -948,25 +921,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="6"/>
@@ -979,25 +952,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="4"/>
@@ -1007,25 +980,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M11" s="5"/>
     </row>
@@ -1034,25 +1007,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J12" s="2"/>
       <c r="L12" s="5"/>
@@ -1063,28 +1036,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="L13" s="2"/>
       <c r="M13" s="5"/>
@@ -1095,25 +1068,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="3"/>
@@ -1124,25 +1097,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J15" s="2"/>
       <c r="M15" s="3"/>
@@ -1152,25 +1125,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M16" s="3"/>
     </row>
@@ -1179,25 +1152,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="3"/>
@@ -1208,25 +1181,25 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="J18" s="2"/>
       <c r="L18" s="8"/>
@@ -1238,25 +1211,25 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="3"/>
@@ -1266,25 +1239,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J20" s="2"/>
       <c r="L20" s="2"/>
@@ -1296,28 +1269,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>35</v>
-      </c>
       <c r="D21" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="N21" s="6"/>
       <c r="P21" s="8"/>
@@ -1325,102 +1298,27 @@
       <c r="R21" s="8"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="3"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="M25" s="3"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>0</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="I26" s="1" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="N27" s="6"/>

</xml_diff>

<commit_message>
fix small error, test commit after moving repository
</commit_message>
<xml_diff>
--- a/blocs/incentives/incentives_info.xlsx
+++ b/blocs/incentives/incentives_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AF81A2-14DE-B549-8426-ADA425BBDC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ACE338-D0E7-4F43-BB8C-3B5193B10AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -661,9 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED89AE72-DC4E-BE45-96E4-63567237423A}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="A22:I26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
bug fixes, updated results
</commit_message>
<xml_diff>
--- a/blocs/incentives/incentives_info.xlsx
+++ b/blocs/incentives/incentives_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Dropbox/Stewart-Guest_Shared/Code/BLocS/blocs/incentives/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daltonwstewart/Documents/Code/BLocS/blocs/incentives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ACE338-D0E7-4F43-BB8C-3B5193B10AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFDDA82-C850-B547-A214-BE6FFF382227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15800" xr2:uid="{07934AD7-5E7F-2741-8249-5F4EF3E42D88}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="95">
   <si>
     <t>property</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Assume compensating tax equivalent to sales tax</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>Assume that value added = FCI</t>
   </si>
   <si>
@@ -257,13 +254,79 @@
   </si>
   <si>
     <t>Capital Investment (Specific Equipment)</t>
+  </si>
+  <si>
+    <t>Code Reference Number</t>
+  </si>
+  <si>
+    <t>Manuscript Reference Number</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,6 +374,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -333,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -343,9 +412,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -661,677 +727,733 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED89AE72-DC4E-BE45-96E4-63567237423A}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N1" s="3"/>
+      <c r="O1" s="4"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="K2" s="2"/>
-      <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L2" s="2"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="5"/>
+      <c r="J3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="L4" s="5"/>
+      <c r="K4" s="2"/>
       <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="H6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10" s="3"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="2"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K12" s="2"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M13" s="2"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="H15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K15" s="2"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L17" s="8"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M17" s="8"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K18" s="2"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="5"/>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M19" s="5"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>69</v>
-      </c>
       <c r="H21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N21" s="6"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="8"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D23" s="2"/>
-      <c r="L23" s="5"/>
+      <c r="O21" s="6"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E23" s="2"/>
       <c r="M23" s="5"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="L24" s="4"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="4"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D25" s="2"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="4"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N27" s="6"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="8"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N28" s="2"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M24" s="4"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="4"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="O27" s="6"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="O28" s="2"/>
-      <c r="Q28" s="5"/>
+      <c r="P28" s="2"/>
+      <c r="R28" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>